<commit_message>
Update this for ritual within Singapore's hotel
</commit_message>
<xml_diff>
--- a/Time Table Apr 2018.xlsx
+++ b/Time Table Apr 2018.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="123">
   <si>
     <t>Time</t>
   </si>
@@ -352,6 +352,39 @@
   <si>
     <t>... วันหยุดเยอะแล้ว เช็คทำไม เดือนหน้าน่ะ</t>
   </si>
+  <si>
+    <t>1 Question is about programmer's oath</t>
+  </si>
+  <si>
+    <t>Questions are very basics</t>
+  </si>
+  <si>
+    <t>Make sure to follow the exercise</t>
+  </si>
+  <si>
+    <t>1 Coding Assignment</t>
+  </si>
+  <si>
+    <t>13:00-24:00</t>
+  </si>
+  <si>
+    <t>Open Anything</t>
+  </si>
+  <si>
+    <t>Go Programming Langauge</t>
+  </si>
+  <si>
+    <t>Go Routine</t>
+  </si>
+  <si>
+    <t>Web Search Engine Mechanism with concurrency</t>
+  </si>
+  <si>
+    <t>Bitcoin Hyperledger</t>
+  </si>
+  <si>
+    <t>Google Cloud Platform</t>
+  </si>
 </sst>
 </file>
 
@@ -495,12 +528,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18997,16 +19030,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>411480</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -19015,8 +19048,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7277100" y="23020020"/>
-          <a:ext cx="1539240" cy="419100"/>
+          <a:off x="7978140" y="22974300"/>
+          <a:ext cx="1135380" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19459,120 +19492,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>411480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="749" name="สี่เหลี่ยมผืนผ้า 748"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11277600" y="3086100"/>
-          <a:ext cx="998220" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ออกกำลัง</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="750" name="สี่เหลี่ยมผืนผ้า 749"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11285220" y="3535680"/>
-          <a:ext cx="982980" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ออกกำลัง</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>502920</xdr:colOff>
       <xdr:row>42</xdr:row>
@@ -21425,63 +21344,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1047" name="สี่เหลี่ยมผืนผ้า 1046"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9212580" y="2651760"/>
-          <a:ext cx="975360" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>เพิ่มปฏิสัมพันธ์กับคนในชมรม</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
       <xdr:row>52</xdr:row>
@@ -22241,16 +22103,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:rowOff>434340</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22259,7 +22121,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14279880" y="18562320"/>
+          <a:off x="15064740" y="22997160"/>
           <a:ext cx="1280160" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22301,16 +22163,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:rowOff>411480</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22319,7 +22181,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13586460" y="18562320"/>
+          <a:off x="14378940" y="22974300"/>
           <a:ext cx="678180" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22586,16 +22448,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>388620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:colOff>220980</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
+      <xdr:rowOff>381000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22604,7 +22466,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6568440" y="22928580"/>
+          <a:off x="5547360" y="23004780"/>
           <a:ext cx="640080" cy="358140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22700,14 +22562,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -22718,7 +22580,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12611100" y="18585180"/>
+          <a:off x="13716000" y="23004780"/>
           <a:ext cx="640080" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22814,73 +22676,73 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:rowOff>396240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1074" name="สี่เหลี่ยมผืนผ้า 1073"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13296900" y="23401020"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1074" name="สี่เหลี่ยมผืนผ้า 1073"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12603480" y="19019520"/>
-          <a:ext cx="640080" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>เดินทาง</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:rowOff>411480</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22889,7 +22751,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12603480" y="19446240"/>
+          <a:off x="13830300" y="23858220"/>
           <a:ext cx="640080" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23042,130 +22904,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>411480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1078" name="สี่เหลี่ยมผืนผ้า 1077"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6149340" y="20764500"/>
-          <a:ext cx="1859280" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>รับผิดชอบบ้าน</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
-            <a:t> ห้อง เสื้อผ้า เพื่อกฏแรงดึงดูด</a:t>
-          </a:r>
-          <a:endParaRPr lang="th-TH" sz="1000"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1079" name="สี่เหลี่ยมผืนผ้า 1078"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6149340" y="21229320"/>
-          <a:ext cx="1874520" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>รับผิดชอบบ้าน</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
-            <a:t> ห้อง เสื้อผ้า เพื่อกฏแรงดึงดูด</a:t>
-          </a:r>
-          <a:endParaRPr lang="th-TH" sz="1000"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
       <xdr:row>55</xdr:row>
@@ -23217,7 +22955,15 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>???</a:t>
+            <a:t>Present Project Web App </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ห้อง </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>503-505</a:t>
           </a:r>
           <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
@@ -23392,6 +23138,9 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -23424,7 +23173,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1000"/>
-            <a:t>Web App</a:t>
+            <a:t>Web App (Workshop)</a:t>
           </a:r>
           <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
@@ -23914,16 +23663,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
       <xdr:row>53</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -23932,7 +23681,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13578840" y="19011900"/>
+          <a:off x="14203680" y="23454360"/>
           <a:ext cx="678180" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23971,14 +23720,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>434340</xdr:rowOff>
     </xdr:to>
@@ -23989,7 +23738,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13594080" y="19461480"/>
+          <a:off x="14851380" y="23881080"/>
           <a:ext cx="678180" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -24489,14 +24238,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>426720</xdr:rowOff>
     </xdr:to>
@@ -24507,7 +24256,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14264640" y="19011900"/>
+          <a:off x="14988540" y="23431500"/>
           <a:ext cx="1303020" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -24556,114 +24305,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1106" name="สี่เหลี่ยมผืนผ้า 1105"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14279880" y="19453860"/>
-          <a:ext cx="1280160" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ศึกษากฏแรงดึงดูด</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1000"/>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>เพื่อ </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Well-Being</a:t>
-          </a:r>
-          <a:endParaRPr lang="th-TH" sz="1000">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="th-TH" sz="1000"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
       <xdr:colOff>411480</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
@@ -25215,16 +24856,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
+      <xdr:rowOff>426720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>411480</xdr:rowOff>
+      <xdr:rowOff>403860</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -25233,7 +24874,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13190220" y="18554700"/>
+          <a:off x="14203680" y="22966680"/>
           <a:ext cx="426720" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -25329,14 +24970,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>419100</xdr:rowOff>
     </xdr:to>
@@ -25347,7 +24988,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13243560" y="19004280"/>
+          <a:off x="13792200" y="23423880"/>
           <a:ext cx="426720" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -25443,16 +25084,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>411480</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -25461,7 +25102,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13159740" y="19438620"/>
+          <a:off x="14447520" y="23888700"/>
           <a:ext cx="426720" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -35990,157 +35631,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="762" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6690360" y="20825460"/>
-          <a:ext cx="1219200" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B050"/>
-        </a:solidFill>
-        <a:ln w="25560">
-          <a:solidFill>
-            <a:srgbClr val="3A5F8B"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>วาดรูปเล่นๆ</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>แวะหาชมรม</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="788" name="สี่เหลี่ยมผืนผ้า 787"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9334500" y="23439120"/>
-          <a:ext cx="1752600" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7030A0"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ไปติดตามผลร้องเรียน</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t> 1111</a:t>
-          </a:r>
-          <a:endParaRPr lang="th-TH" sz="1000"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
@@ -36209,13 +35699,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
+      <xdr:colOff>373380</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>434340</xdr:rowOff>
     </xdr:to>
@@ -36226,7 +35716,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12519660" y="20787360"/>
+          <a:off x="12306300" y="20787360"/>
           <a:ext cx="1432560" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -36273,16 +35763,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>403860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -36291,8 +35781,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12603480" y="21198840"/>
-          <a:ext cx="1432560" cy="419100"/>
+          <a:off x="12534900" y="23385780"/>
+          <a:ext cx="883920" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -37140,6 +36630,1537 @@
             <a:t>ตึกคอมไฟดับ</a:t>
           </a:r>
           <a:endParaRPr sz="800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="816" name="สี่เหลี่ยมผืนผ้า 815"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9105900" y="20353020"/>
+          <a:ext cx="1104900" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ทำงานกลุ่ม </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="817" name="สี่เหลี่ยมผืนผ้า 816"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7231380" y="20787360"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>426720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>403860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="818" name="สี่เหลี่ยมผืนผ้า 817"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7277100" y="21198840"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="819" name="สี่เหลี่ยมผืนผ้า 818"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10081260" y="23416260"/>
+          <a:ext cx="1104900" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>มาดูงานกลุ่ม</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="820" name="สี่เหลี่ยมผืนผ้า 819"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10370820" y="20772120"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="821" name="สี่เหลี่ยมผืนผ้า 820"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13479780" y="21244560"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>144300</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>411060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="788" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5638800" y="24757380"/>
+          <a:ext cx="471960" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="822" name="สี่เหลี่ยมผืนผ้า 821"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8549640" y="23858220"/>
+          <a:ext cx="762000" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>อาหารฟรีที่กองกิจ</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="823" name="สี่เหลี่ยมผืนผ้า 822"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5974080" y="20772120"/>
+          <a:ext cx="1432560" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ติว </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Com Security</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="825" name="สี่เหลี่ยมผืนผ้า 824"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6347460" y="23012400"/>
+          <a:ext cx="1417320" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ทำงานกลุ่ม </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="826" name="สี่เหลี่ยมผืนผ้า 825"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11033760" y="21214080"/>
+          <a:ext cx="1104900" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ทำงานกลุ่ม </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="827" name="สี่เหลี่ยมผืนผ้า 826"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11041380" y="20787360"/>
+          <a:ext cx="1104900" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ทำงานกลุ่ม </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="828" name="สี่เหลี่ยมผืนผ้า 827"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5913120" y="21206460"/>
+          <a:ext cx="1432560" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ติว </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Tech Write</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="749" name="สี่เหลี่ยมผืนผ้า 748"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12207240" y="21236940"/>
+          <a:ext cx="1432560" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ติว </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Com Security</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="750" name="สี่เหลี่ยมผืนผ้า 749"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15407640" y="21206460"/>
+          <a:ext cx="1104900" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ทำงานกลุ่ม </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>426720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>167160</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>388200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="762" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4998720" y="22966680"/>
+          <a:ext cx="471960" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>411000</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>403440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="824" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4579620" y="23865840"/>
+          <a:ext cx="471960" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>426720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="830" name="สี่เหลี่ยมผืนผ้า 829"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12656820" y="23873460"/>
+          <a:ext cx="883920" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ติว </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Lab Phy II</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="833" name="สี่เหลี่ยมผืนผ้า 832"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15400020" y="23888700"/>
+          <a:ext cx="1104900" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ประสานงาน </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="829" name="สี่เหลี่ยมผืนผ้า 828"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5646420" y="23881080"/>
+          <a:ext cx="975360" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เพิ่มปฏิสัมพันธ์กับคนในชมรม</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>388620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="831" name="สี่เหลี่ยมผืนผ้า 830"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8808720" y="23393400"/>
+          <a:ext cx="1280160" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เอาผลบันทึก </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Lab PHy II </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ที่ตึกวิทย์ ชั้น </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>6</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="832" name="สี่เหลี่ยมผืนผ้า 831"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6789420" y="25222200"/>
+          <a:ext cx="1104900" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="700"/>
+            <a:t>Check</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="700" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="700" baseline="0"/>
+            <a:t>ที่อยู่ของ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="700" baseline="0"/>
+            <a:t>SuperRich1965 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="700" baseline="0"/>
+            <a:t>ที่ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="700" baseline="0"/>
+            <a:t>CenLad</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="700"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>388620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="834" name="สี่เหลี่ยมผืนผ้า 833"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6088380" y="25161240"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="835" name="สี่เหลี่ยมผืนผ้า 834"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6118860" y="25633680"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -59409,10 +60430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1000"/>
+  <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="N56" sqref="N56"/>
+    <sheetView tabSelected="1" topLeftCell="F48" workbookViewId="0">
+      <selection activeCell="U40" sqref="U40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -59424,32 +60445,32 @@
       <c r="A1" s="1">
         <v>43191</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="13"/>
     </row>
     <row r="2" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -59743,32 +60764,32 @@
       <c r="A11" s="1">
         <v>43191</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="13"/>
     </row>
     <row r="12" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -60057,32 +61078,32 @@
       <c r="A21" s="1">
         <v>43191</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="13"/>
     </row>
     <row r="22" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -60387,32 +61408,32 @@
       <c r="A31" s="1">
         <v>43191</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="12"/>
+      <c r="W31" s="12"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="13"/>
     </row>
     <row r="32" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -60703,32 +61724,32 @@
       <c r="A41" s="1">
         <v>43191</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-      <c r="T41" s="11"/>
-      <c r="U41" s="11"/>
-      <c r="V41" s="11"/>
-      <c r="W41" s="11"/>
-      <c r="X41" s="11"/>
-      <c r="Y41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+      <c r="S41" s="12"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="12"/>
+      <c r="V41" s="12"/>
+      <c r="W41" s="12"/>
+      <c r="X41" s="12"/>
+      <c r="Y41" s="13"/>
     </row>
     <row r="42" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -61021,32 +62042,32 @@
       <c r="A51" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="11"/>
-      <c r="T51" s="11"/>
-      <c r="U51" s="11"/>
-      <c r="V51" s="11"/>
-      <c r="W51" s="11"/>
-      <c r="X51" s="11"/>
-      <c r="Y51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+      <c r="S51" s="12"/>
+      <c r="T51" s="12"/>
+      <c r="U51" s="12"/>
+      <c r="V51" s="12"/>
+      <c r="W51" s="12"/>
+      <c r="X51" s="12"/>
+      <c r="Y51" s="13"/>
     </row>
     <row r="52" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
@@ -61349,7 +62370,7 @@
       <c r="C64" t="s">
         <v>92</v>
       </c>
-      <c r="E64" s="13">
+      <c r="E64" s="10">
         <v>43216</v>
       </c>
       <c r="G64" t="s">
@@ -61362,11 +62383,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="65" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>95</v>
       </c>
-      <c r="E65" s="13">
+      <c r="E65" s="10">
         <v>43221</v>
       </c>
       <c r="G65" t="s">
@@ -61379,11 +62400,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>98</v>
       </c>
-      <c r="E66" s="13">
+      <c r="E66" s="10">
         <v>43222</v>
       </c>
       <c r="G66" t="s">
@@ -61396,11 +62417,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="67" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>99</v>
       </c>
-      <c r="E67" s="13">
+      <c r="E67" s="10">
         <v>43223</v>
       </c>
       <c r="G67" t="s">
@@ -61413,11 +62434,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>101</v>
       </c>
-      <c r="E68" s="13">
+      <c r="E68" s="10">
         <v>43231</v>
       </c>
       <c r="G68" t="s">
@@ -61430,11 +62451,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="69" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>102</v>
       </c>
-      <c r="E69" s="13">
+      <c r="E69" s="10">
         <v>43231</v>
       </c>
       <c r="G69" t="s">
@@ -61447,15 +62468,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="70" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>103</v>
       </c>
-      <c r="E70" s="13">
+      <c r="E70" s="10">
         <v>43227</v>
       </c>
       <c r="G70" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="I70" t="s">
         <v>94</v>
@@ -61463,12 +62484,42 @@
       <c r="K70" t="s">
         <v>108</v>
       </c>
+      <c r="M70" t="s">
+        <v>117</v>
+      </c>
+      <c r="O70" t="s">
+        <v>112</v>
+      </c>
+      <c r="S70" t="s">
+        <v>113</v>
+      </c>
+      <c r="V70" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE70" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI70" t="s">
+        <v>121</v>
+      </c>
+      <c r="AK70" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="71" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>104</v>
       </c>
-      <c r="E71" s="13">
+      <c r="E71" s="10">
         <v>43235</v>
       </c>
       <c r="G71" t="s">
@@ -61481,15 +62532,15 @@
         <v>109</v>
       </c>
     </row>
-    <row r="72" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="3:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="3:37" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -62439,32 +63490,32 @@
       <c r="A1" s="1">
         <v>43191</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="13"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -62755,32 +63806,32 @@
       <c r="A11" s="1">
         <v>43160</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="13"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -63066,32 +64117,32 @@
       <c r="A21" s="1">
         <v>43160</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="13"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -63377,32 +64428,32 @@
       <c r="A31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="12"/>
+      <c r="W31" s="12"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="13"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">

</xml_diff>

<commit_message>
Added May 2018 version
</commit_message>
<xml_diff>
--- a/Time Table Apr 2018.xlsx
+++ b/Time Table Apr 2018.xlsx
@@ -22391,16 +22391,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22409,7 +22409,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6629400" y="19895820"/>
+          <a:off x="7917180" y="24330660"/>
           <a:ext cx="640080" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22505,14 +22505,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -22523,7 +22523,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13639800" y="19911060"/>
+          <a:off x="14340840" y="24330660"/>
           <a:ext cx="640080" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -22619,63 +22619,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1073" name="สี่เหลี่ยมผืนผ้า 1072"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15171420" y="19903440"/>
-          <a:ext cx="807720" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ศึกษากฏแรงดึงดูด</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>52</xdr:row>
@@ -22790,16 +22733,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>55517</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>418010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>32657</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
+      <xdr:rowOff>390796</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22808,8 +22751,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12618720" y="20345400"/>
-          <a:ext cx="640080" cy="419100"/>
+          <a:off x="14664146" y="24965296"/>
+          <a:ext cx="641168" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -23183,63 +23126,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>632460</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1086" name="สี่เหลี่ยมผืนผ้า 1085"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10218420" y="20330160"/>
-          <a:ext cx="1021080" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>แวะหา กองกิจ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>53</xdr:row>
@@ -23362,63 +23248,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1089" name="สี่เหลี่ยมผืนผ้า 1088"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11285220" y="20337780"/>
-          <a:ext cx="960120" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ออกกำลัง</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>45720</xdr:colOff>
       <xdr:row>55</xdr:row>
@@ -23550,13 +23379,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:colOff>434340</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>434340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>411480</xdr:rowOff>
     </xdr:to>
@@ -23567,65 +23396,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11277600" y="20764500"/>
+          <a:off x="11704320" y="25184100"/>
           <a:ext cx="998220" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ออกกำลัง</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1093" name="สี่เหลี่ยมผืนผ้า 1092"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11285220" y="21214080"/>
-          <a:ext cx="982980" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -23777,25 +23549,139 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>463732</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:rowOff>8709</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>478972</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>432163</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1096" name="สี่เหลี่ยมผืนผ้า 1095"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15736389" y="25002309"/>
+          <a:ext cx="679269" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>สวดมนต์</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>426720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1097" name="สี่เหลี่ยมผืนผ้า 1096"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15384780" y="24315420"/>
+          <a:ext cx="640080" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>สวดมนต์</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1096" name="สี่เหลี่ยมผืนผ้า 1095"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13624560" y="20360640"/>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1098" name="สี่เหลี่ยมผืนผ้า 1097"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14607540" y="25191720"/>
           <a:ext cx="678180" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23835,129 +23721,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1097" name="สี่เหลี่ยมผืนผ้า 1096"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14584680" y="19888200"/>
-          <a:ext cx="640080" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>สวดมนต์</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1098" name="สี่เหลี่ยมผืนผ้า 1097"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12931140" y="20787360"/>
-          <a:ext cx="678180" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>สวดมนต์</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
+      <xdr:rowOff>411480</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -23966,7 +23738,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12900660" y="21221700"/>
+          <a:off x="14630400" y="25626060"/>
           <a:ext cx="678180" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -24304,63 +24076,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1107" name="สี่เหลี่ยมผืนผ้า 1106"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14333220" y="20353020"/>
-          <a:ext cx="1280160" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ศึกษากฏแรงดึงดูด</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>57</xdr:row>
@@ -24423,344 +24138,82 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>632460</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1114" name="สี่เหลี่ยมผืนผ้า 1113"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15278100" y="25184100"/>
+          <a:ext cx="967740" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ตรวจปฎิทิน</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1110" name="สี่เหลี่ยมผืนผ้า 1109"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9250680" y="20794980"/>
-          <a:ext cx="2004060" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t>Check </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>การบ้าน งาน ให้ดีๆ ถ้ามีก็ทำ</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
-            <a:t> ถ้าไม่มีก็แวะที่ทำงานใหม่</a:t>
-          </a:r>
-          <a:endParaRPr lang="th-TH" sz="1000"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1111" name="สี่เหลี่ยมผืนผ้า 1110"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9258300" y="21229320"/>
-          <a:ext cx="2004060" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t>Check </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>การบ้าน งาน ให้ดีๆ ถ้ามีก็ทำ</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
-            <a:t> ถ้าไม่มีก็แวะบ้านใหม่</a:t>
-          </a:r>
-          <a:endParaRPr lang="th-TH" sz="1000"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1112" name="สี่เหลี่ยมผืนผ้า 1111"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13571220" y="20794980"/>
-          <a:ext cx="1379220" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ศึกษากฏแรงดึงดูด</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ด้วยการประยุกต์</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1113" name="สี่เหลี่ยมผืนผ้า 1112"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13578840" y="21229320"/>
-          <a:ext cx="1417320" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ศึกษากฏแรงดึงดูด</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ด้วยการประยุกต์</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>57</xdr:row>
       <xdr:rowOff>426720</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1114" name="สี่เหลี่ยมผืนผ้า 1113"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14935200" y="20779740"/>
-          <a:ext cx="967740" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ตรวจปฎิทิน</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>434340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>411480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
         <xdr:cNvPr id="1115" name="สี่เหลี่ยมผืนผ้า 1114"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14965680" y="21206460"/>
+          <a:off x="15354300" y="25641300"/>
           <a:ext cx="937260" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -25198,197 +24651,311 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1123" name="สี่เหลี่ยมผืนผ้า 1122"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14211300" y="19888200"/>
-          <a:ext cx="426720" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>อาบน้ำ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>403860</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1124" name="สี่เหลี่ยมผืนผ้า 1123"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12230100" y="20314920"/>
-          <a:ext cx="396240" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>กินข้าวแ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>632460</xdr:colOff>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>411480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1123" name="สี่เหลี่ยมผืนผ้า 1122"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14958060" y="24300180"/>
+          <a:ext cx="426720" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>อาบน้ำ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>340722</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>34834</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>74022</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>11974</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1124" name="สี่เหลี่ยมผืนผ้า 1123"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14285322" y="25028434"/>
+          <a:ext cx="397329" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>กินข้าวแ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>55518</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>8708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>483326</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>432162</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1125" name="สี่เหลี่ยมผืนผ้า 1124"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15328175" y="25002308"/>
+          <a:ext cx="427808" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>อาบน้ำ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>388620</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1125" name="สี่เหลี่ยมผืนผ้า 1124"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13228320" y="20299680"/>
-          <a:ext cx="426720" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>อาบน้ำ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:colOff>441960</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1126" name="สี่เหลี่ยมผืนผ้า 1125"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13700760" y="25191720"/>
+          <a:ext cx="396240" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>กินข้าวแ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1126" name="สี่เหลี่ยมผืนผ้า 1125"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12199620" y="20779740"/>
-          <a:ext cx="396240" cy="419100"/>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1127" name="สี่เหลี่ยมผืนผ้า 1126"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14157960" y="25191720"/>
+          <a:ext cx="426720" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>อาบน้ำ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>34834</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>11975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1128" name="สี่เหลี่ยมผืนผ้า 1127"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12379234" y="25921063"/>
+          <a:ext cx="397329" cy="423455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -25426,130 +24993,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>426720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1127" name="สี่เหลี่ยมผืนผ้า 1126"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12542520" y="20779740"/>
-          <a:ext cx="426720" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>อาบน้ำ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1128" name="สี่เหลี่ยมผืนผ้า 1127"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12199620" y="21214080"/>
-          <a:ext cx="396240" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>กินข้าวแ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:rowOff>403860</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -25558,7 +25011,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12542520" y="21214080"/>
+          <a:off x="14142720" y="25618440"/>
           <a:ext cx="426720" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -25703,63 +25156,6 @@
           <a:r>
             <a:rPr lang="th-TH" sz="1000"/>
             <a:t>เพิ่มปฏิสัมพันธ์กับคนในบ้าน</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1132" name="สี่เหลี่ยมผืนผ้า 1131"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9212580" y="20330160"/>
-          <a:ext cx="975360" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>เพิ่มปฏิสัมพันธ์กับคนในชมรม</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -27074,8 +26470,8 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>232140</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>418800</xdr:rowOff>
     </xdr:to>
@@ -27087,7 +26483,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7985760" y="25206960"/>
-          <a:ext cx="2853420" cy="403560"/>
+          <a:ext cx="1912620" cy="403560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -27150,8 +26546,8 @@
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>277860</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>434040</xdr:rowOff>
     </xdr:to>
@@ -27163,7 +26559,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8031480" y="25664160"/>
-          <a:ext cx="2853420" cy="403560"/>
+          <a:ext cx="1813560" cy="403560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -37707,16 +37103,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
+      <xdr:rowOff>396240</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -37725,7 +37121,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12656820" y="23873460"/>
+          <a:off x="16664940" y="23842980"/>
           <a:ext cx="883920" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -37772,16 +37168,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>411480</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -37790,7 +37186,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15400020" y="23888700"/>
+          <a:off x="12633960" y="23858220"/>
           <a:ext cx="1104900" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -37971,14 +37367,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>453935</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>231865</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
@@ -37989,8 +37385,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6789420" y="25222200"/>
-          <a:ext cx="1104900" cy="419100"/>
+          <a:off x="9086306" y="25470394"/>
+          <a:ext cx="1105988" cy="423455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -38112,25 +37508,931 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>424544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
       <xdr:row>58</xdr:row>
+      <xdr:rowOff>397329</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="835" name="สี่เหลี่ยมผืนผ้า 834"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6052457" y="25864458"/>
+          <a:ext cx="641169" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="836" name="สี่เหลี่ยมผืนผ้า 835"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15293340" y="23888700"/>
+          <a:ext cx="1424940" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Test Push </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ลง </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Com </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เล็ก </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>(Web App)</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="837" name="สี่เหลี่ยมผืนผ้า 836"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6606540" y="24330660"/>
+          <a:ext cx="1104900" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ประสานงาน </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>434340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>517680</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>395820</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="838" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5349240" y="24300180"/>
+          <a:ext cx="471960" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50074</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>17417</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>631372</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>420977</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="839" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8682445" y="25011017"/>
+          <a:ext cx="5229498" cy="403560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ปรึกษาการใช้</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Vue.js </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ทำ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Front-end </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>กับ อ.ภารุจ หรือคนอื่นๆ ที่มี</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ให้ปรางถามการเชื่อมด้วย</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>***CRITICAL*** </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ตัวกำหนดชะตาวิชา </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Web App Dev </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>เลย คอยถามอาจารย์ไว้</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ถ้าถามไม่ได้ ก็ดรอปแม่ง</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>435429</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>3266</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>244449</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>406706</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="840" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5747658" y="25443180"/>
+          <a:ext cx="473048" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>627017</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>29392</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>404948</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="835" name="สี่เหลี่ยมผืนผ้า 834"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6118860" y="25633680"/>
-          <a:ext cx="640080" cy="419100"/>
+      <xdr:rowOff>6531</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="841" name="สี่เหลี่ยมผืนผ้า 840"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10587446" y="25469306"/>
+          <a:ext cx="1105988" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ประสานงาน </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>290647</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>174171</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>3266</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="842" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11579133" y="25508495"/>
+          <a:ext cx="1211581" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>เล่นเกมส์</a:t>
+          </a:r>
+          <a:endParaRPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>14152</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>261257</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>437606</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="843" name="สี่เหลี่ยมผืนผ้า 842"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16203386" y="25454066"/>
+          <a:ext cx="1322614" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ติว </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Go Programming</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>Soft PAt</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>391886</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>46808</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>631371</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>23948</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="844" name="สี่เหลี่ยมผืนผ้า 843"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6368143" y="25933037"/>
+          <a:ext cx="1567542" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ติว </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t> Cloud Dataflow</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> Big Data , Docker </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>Soft PAt</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>604156</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>3265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>348343</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>426719</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="845" name="สี่เหลี่ยมผืนผ้า 844"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10564585" y="25889494"/>
+          <a:ext cx="1736272" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ติว </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t> Naist and Machine Learning</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>Soft PAt</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>610688</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>30479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>587828</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>3265</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="846" name="สี่เหลี่ยมผืนผ้า 845"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9907088" y="25916708"/>
+          <a:ext cx="641169" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -38161,6 +38463,73 @@
             <a:rPr lang="th-TH" sz="1000"/>
             <a:t>เดินทาง</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>507274</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>18505</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>285205</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>441959</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="847" name="สี่เหลี่ยมผืนผ้า 846"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13123817" y="25904734"/>
+          <a:ext cx="1105988" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ประสานงาน </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Web App</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -60432,8 +60801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F48" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>